<commit_message>
Atualize o programa de criação de planilha de acordo com o modelo
</commit_message>
<xml_diff>
--- a/openpyxl/Carteira Cláudia.xlsx
+++ b/openpyxl/Carteira Cláudia.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Dashboard" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dashboard" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,8 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="R$#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="R#,##0.00"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,6 +30,15 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,14 +61,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,117 +439,252 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:F9"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="27" customWidth="1" min="1" max="1"/>
+    <col width="27" customWidth="1" min="2" max="2"/>
+    <col width="27" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="27" customWidth="1" min="5" max="5"/>
+    <col width="27" customWidth="1" min="6" max="6"/>
+    <col width="27" customWidth="1" min="7" max="7"/>
+    <col width="27" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
-    <row r="2">
-      <c r="B2" s="1" t="inlineStr">
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Resumo da Carteira</t>
         </is>
       </c>
     </row>
-    <row r="3"/>
-    <row r="4">
-      <c r="B4" t="inlineStr">
+    <row r="2" ht="27" customHeight="1"/>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Ações</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>Moedas</t>
         </is>
       </c>
     </row>
+    <row r="4"/>
     <row r="5">
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Valor da ação (R$)</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Valor acumulado (R$)</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>Valor da ação (R$)</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>Valor acumulado (R$)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>VALE3</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="B6" t="n">
         <v>1000</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="C6" s="4" t="n">
+        <v>84.25</v>
+      </c>
+      <c r="D6" s="4">
+        <f>B6*C6</f>
+        <v/>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>CAD</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="F6" t="n">
         <v>150</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
+      <c r="G6" s="5" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="H6" s="5">
+        <f>F6*G6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>MGLU3</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="B7" t="n">
         <v>1000</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="C7" s="4" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="D7" s="4">
+        <f>B7*C7</f>
+        <v/>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>CHF</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="F7" t="n">
         <v>500</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
+      <c r="G7" s="5" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="H7" s="5">
+        <f>F7*G7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>ITUB4</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="B8" t="n">
         <v>375</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="C8" s="4" t="n">
+        <v>26.02</v>
+      </c>
+      <c r="D8" s="4">
+        <f>B8*C8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>Total Ações</t>
+        </is>
+      </c>
+      <c r="B9">
+        <f>SUM(B6:B8)</f>
+        <v/>
+      </c>
+      <c r="C9" s="5">
+        <f>SUM(C6:C8)</f>
+        <v/>
+      </c>
+      <c r="D9" s="5">
+        <f>SUM(D6:D8)</f>
+        <v/>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
         <is>
           <t>Total Moedas</t>
         </is>
       </c>
-      <c r="E7">
-        <f>SUM(E5:E6)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Total Ações</t>
-        </is>
-      </c>
-      <c r="C8">
-        <f>SUM(C5:C7)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>TOTAL:</t>
-        </is>
-      </c>
       <c r="F9">
-        <f>SUM(C5:C7) + SUM(E5:E6)</f>
+        <f>SUM(F6:F8)</f>
+        <v/>
+      </c>
+      <c r="G9" s="5">
+        <f>SUM(G6:G8)</f>
+        <v/>
+      </c>
+      <c r="H9" s="5">
+        <f>SUM(H6:H8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>Valor da Carteira</t>
+        </is>
+      </c>
+    </row>
+    <row r="13"/>
+    <row r="14">
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>Valor acumulado total (R$)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" s="5">
+        <f>B9+F9</f>
+        <v/>
+      </c>
+      <c r="E15" s="5">
+        <f>D9+H9</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B9:E9"/>
+  <mergeCells count="16">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="A5"/>
+    <mergeCell ref="B5"/>
+    <mergeCell ref="C5"/>
+    <mergeCell ref="D5"/>
+    <mergeCell ref="E3:H4"/>
+    <mergeCell ref="E5"/>
+    <mergeCell ref="F5"/>
+    <mergeCell ref="G5"/>
+    <mergeCell ref="H5"/>
+    <mergeCell ref="A9"/>
+    <mergeCell ref="E9"/>
+    <mergeCell ref="D12:E13"/>
+    <mergeCell ref="D14"/>
+    <mergeCell ref="E14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrija a formatação de números em dados financeiros
</commit_message>
<xml_diff>
--- a/openpyxl/Carteira Cláudia.xlsx
+++ b/openpyxl/Carteira Cláudia.xlsx
@@ -16,9 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="R$#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="R#,##0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -61,7 +60,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -73,7 +72,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -544,10 +542,10 @@
       <c r="F6" t="n">
         <v>150</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="4" t="n">
         <v>3.74</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <f>F6*G6</f>
         <v/>
       </c>
@@ -576,10 +574,10 @@
       <c r="F7" t="n">
         <v>500</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="4" t="n">
         <v>4.97</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <f>F7*G7</f>
         <v/>
       </c>
@@ -611,11 +609,11 @@
         <f>SUM(B6:B8)</f>
         <v/>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <f>SUM(C6:C8)</f>
         <v/>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <f>SUM(D6:D8)</f>
         <v/>
       </c>
@@ -628,11 +626,11 @@
         <f>SUM(F6:F8)</f>
         <v/>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <f>SUM(G6:G8)</f>
         <v/>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <f>SUM(H6:H8)</f>
         <v/>
       </c>
@@ -658,11 +656,11 @@
       </c>
     </row>
     <row r="15">
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <f>B9+F9</f>
         <v/>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <f>D9+H9</f>
         <v/>
       </c>

</xml_diff>